<commit_message>
remove and replace photos 3
</commit_message>
<xml_diff>
--- a/docs/portfolio.xlsx
+++ b/docs/portfolio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ecc85ccb002dd88c/Projects/mooremanordesigns.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{F5B818F5-FA86-4F87-A408-A48E3EF64669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E2D3F20-7320-47AA-92F0-832DADE3E733}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{F5B818F5-FA86-4F87-A408-A48E3EF64669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15C04EF4-E6D5-4C30-978A-8B3947DAA745}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{436361DF-52DD-460D-9FB3-3363FA009BCD}"/>
   </bookViews>
@@ -1061,7 +1061,79 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <color theme="1" tint="0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <color theme="1" tint="0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <color theme="1" tint="0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1145,18 +1217,6 @@
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1177,36 +1237,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BEC4E9FD-2B38-4FC7-8049-9023C5F715E4}" name="Paintings.Table" displayName="Paintings.Table" ref="A1:R124" totalsRowShown="0" headerRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BEC4E9FD-2B38-4FC7-8049-9023C5F715E4}" name="portfolio.table" displayName="portfolio.table" ref="A1:R124" totalsRowShown="0" headerRowDxfId="27">
   <autoFilter ref="A1:R124" xr:uid="{23143FBE-2AF4-46A6-9F78-52A9759D713F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R124">
     <sortCondition ref="B2:B124"/>
     <sortCondition ref="A2:A124"/>
   </sortState>
   <tableColumns count="18">
-    <tableColumn id="9" xr3:uid="{5B7A858D-E5C0-47C8-95F1-29BE364D59D1}" name="Filename" dataDxfId="15">
-      <calculatedColumnFormula>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</calculatedColumnFormula>
+    <tableColumn id="9" xr3:uid="{5B7A858D-E5C0-47C8-95F1-29BE364D59D1}" name="Filename" dataDxfId="26">
+      <calculatedColumnFormula>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{1C22BD59-9C25-4F2C-8884-72C883A837B1}" name="Include" dataDxfId="14">
-      <calculatedColumnFormula>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</calculatedColumnFormula>
+    <tableColumn id="14" xr3:uid="{1C22BD59-9C25-4F2C-8884-72C883A837B1}" name="Include" dataDxfId="25">
+      <calculatedColumnFormula>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="1" xr3:uid="{7DF0D842-9A07-4F32-9A22-C88E5853ED33}" name="Category"/>
     <tableColumn id="2" xr3:uid="{BC061CA4-BDC5-44BA-B403-ACD105A38E6A}" name="Series"/>
-    <tableColumn id="3" xr3:uid="{B7D64594-94CF-4D23-B1E1-CF59D686B1F3}" name="Title" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{4D7F8670-91BB-40FA-B49C-62566B0B2CAB}" name="Year" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{B7D64594-94CF-4D23-B1E1-CF59D686B1F3}" name="Title" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{4D7F8670-91BB-40FA-B49C-62566B0B2CAB}" name="Year" dataDxfId="23"/>
     <tableColumn id="4" xr3:uid="{3F8A6B28-1093-4693-9FF7-6105AED8534B}" name="Width"/>
     <tableColumn id="5" xr3:uid="{72C2B875-E7D6-4BB5-9FE4-1B38EF88FD7B}" name="Length"/>
-    <tableColumn id="6" xr3:uid="{86825EB6-C340-453B-A16A-48B0274F4965}" name="Dimensions" dataDxfId="11">
-      <calculatedColumnFormula>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{86825EB6-C340-453B-A16A-48B0274F4965}" name="Dimensions" dataDxfId="22">
+      <calculatedColumnFormula>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{D204B81F-B1E3-4F84-9E11-6A7F96BA5521}" name="Framed" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{CF043A25-5602-4987-9A50-FBE0E6A6FF6D}" name="Price.Ask" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{283168F4-2468-43CB-BD60-5AD97027893C}" name="Price.List" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{649C86E1-9495-4246-BAC2-CED30A646F0F}" name="Price.Sale" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{F2298965-3AF1-4CB7-A947-2BC83C4B3530}" name="Price.Status.Notes" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{836D4801-5D71-4595-97A7-D202ACE67724}" name="Status.Sale" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{0715EB14-7918-456A-8D07-251FC53FEF2B}" name="Status.Post" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{C475F84E-A8C2-4675-96A9-370E4BE697BD}" name="Status.Photo" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{D204B81F-B1E3-4F84-9E11-6A7F96BA5521}" name="Framed" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{CF043A25-5602-4987-9A50-FBE0E6A6FF6D}" name="Price.Ask" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{283168F4-2468-43CB-BD60-5AD97027893C}" name="Price.List" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{649C86E1-9495-4246-BAC2-CED30A646F0F}" name="Price.Sale" dataDxfId="18"/>
+    <tableColumn id="15" xr3:uid="{F2298965-3AF1-4CB7-A947-2BC83C4B3530}" name="Price.Status.Notes" dataDxfId="17"/>
+    <tableColumn id="13" xr3:uid="{836D4801-5D71-4595-97A7-D202ACE67724}" name="Status.Sale" dataDxfId="16"/>
+    <tableColumn id="16" xr3:uid="{0715EB14-7918-456A-8D07-251FC53FEF2B}" name="Status.Post" dataDxfId="15"/>
+    <tableColumn id="17" xr3:uid="{C475F84E-A8C2-4675-96A9-370E4BE697BD}" name="Status.Photo" dataDxfId="14"/>
     <tableColumn id="10" xr3:uid="{5326519F-F06A-4075-A35A-AA69D194CDB1}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1214,7 +1274,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5DDE0F4D-CD7D-42F0-AAD4-99E4FD427C88}" name="Category.Table" displayName="Category.Table" ref="A1:A9" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5DDE0F4D-CD7D-42F0-AAD4-99E4FD427C88}" name="Category.Table" displayName="Category.Table" ref="A1:A9" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A1:A9" xr:uid="{535629D5-D5B3-4151-81E7-AC9A74A5ED01}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A7">
     <sortCondition ref="A1:A7"/>
@@ -1227,7 +1287,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7802B257-70CD-41BB-AFBF-5480702F402C}" name="Subcategory.Table" displayName="Subcategory.Table" ref="C1:I7" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7802B257-70CD-41BB-AFBF-5480702F402C}" name="Subcategory.Table" displayName="Subcategory.Table" ref="C1:I7" totalsRowShown="0" headerRowDxfId="12">
   <autoFilter ref="C1:I7" xr:uid="{08463D02-E487-4EEB-A80C-CA4F702068E6}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{A1231EA8-3C3E-4975-B930-61C0B93A50E2}" name="Portait"/>
@@ -1243,7 +1303,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BBDF68BD-D421-487E-94D4-D0F9FDD9892F}" name="Status.Table" displayName="Status.Table" ref="K1:M7" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BBDF68BD-D421-487E-94D4-D0F9FDD9892F}" name="Status.Table" displayName="Status.Table" ref="K1:M7" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="K1:M7" xr:uid="{7597EB04-335A-4658-9C5E-54700C2640F3}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E3C3437E-D4C6-46B5-A846-07B0F64A27ED}" name="Status.Sale"/>
@@ -1561,9 +1621,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFDEB908-3F7F-458A-B166-08C443129F53}">
   <dimension ref="A1:R124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P49" sqref="P49"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K112" sqref="K112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1646,11 +1706,11 @@
     </row>
     <row r="2" spans="1:18" s="6" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Abstract_Corruption</v>
       </c>
       <c r="B2" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>No</v>
       </c>
       <c r="C2" t="s">
@@ -1670,7 +1730,7 @@
         <v>48</v>
       </c>
       <c r="I2" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x48</v>
       </c>
       <c r="J2" s="11" t="s">
@@ -1695,11 +1755,11 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Abstract_Cosmic</v>
       </c>
       <c r="B3" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>No</v>
       </c>
       <c r="C3" t="s">
@@ -1710,7 +1770,7 @@
       </c>
       <c r="F3" s="10"/>
       <c r="I3" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J3" s="11" t="s">
@@ -1730,11 +1790,11 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Abstract_Sunburst</v>
       </c>
       <c r="B4" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>No</v>
       </c>
       <c r="C4" t="s">
@@ -1745,7 +1805,7 @@
       </c>
       <c r="F4" s="10"/>
       <c r="I4" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J4" s="11" t="s">
@@ -1765,11 +1825,11 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_Dragonfly</v>
       </c>
       <c r="B5" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>No</v>
       </c>
       <c r="C5" t="s">
@@ -1780,7 +1840,7 @@
       </c>
       <c r="F5" s="10"/>
       <c r="I5" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J5" s="11" t="s">
@@ -1803,11 +1863,11 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_Galen</v>
       </c>
       <c r="B6" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>No</v>
       </c>
       <c r="C6" t="s">
@@ -1820,7 +1880,7 @@
         <v>2020</v>
       </c>
       <c r="I6" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J6" s="11" t="s">
@@ -1845,11 +1905,11 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_LeanonMe</v>
       </c>
       <c r="B7" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>No</v>
       </c>
       <c r="C7" t="s">
@@ -1860,7 +1920,7 @@
       </c>
       <c r="F7" s="10"/>
       <c r="I7" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J7" s="11" t="s">
@@ -1883,11 +1943,11 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_Majestic</v>
       </c>
       <c r="B8" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>No</v>
       </c>
       <c r="C8" t="s">
@@ -1898,7 +1958,7 @@
       </c>
       <c r="F8" s="10"/>
       <c r="I8" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J8" s="11" t="s">
@@ -1921,11 +1981,11 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_Milos</v>
       </c>
       <c r="B9" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>No</v>
       </c>
       <c r="C9" t="s">
@@ -1936,7 +1996,7 @@
       </c>
       <c r="F9" s="10"/>
       <c r="I9" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J9" s="11" t="s">
@@ -1959,11 +2019,11 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_NeverForgetFernanda</v>
       </c>
       <c r="B10" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>No</v>
       </c>
       <c r="C10" t="s">
@@ -1974,7 +2034,7 @@
       </c>
       <c r="F10" s="10"/>
       <c r="I10" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J10" s="11" t="s">
@@ -1997,11 +2057,11 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_Puppy</v>
       </c>
       <c r="B11" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>No</v>
       </c>
       <c r="C11" t="s">
@@ -2012,7 +2072,7 @@
       </c>
       <c r="F11" s="10"/>
       <c r="I11" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J11" s="11" t="s">
@@ -2035,11 +2095,11 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_Serenity</v>
       </c>
       <c r="B12" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>No</v>
       </c>
       <c r="C12" t="s">
@@ -2050,7 +2110,7 @@
       </c>
       <c r="F12" s="10"/>
       <c r="I12" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J12" s="11" t="s">
@@ -2070,11 +2130,11 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Comics_Carnage</v>
       </c>
       <c r="B13" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>No</v>
       </c>
       <c r="C13" t="s">
@@ -2087,7 +2147,7 @@
         <v>2021</v>
       </c>
       <c r="I13" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J13" s="11" t="s">
@@ -2107,11 +2167,11 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Comics_IronMan</v>
       </c>
       <c r="B14" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>No</v>
       </c>
       <c r="C14" t="s">
@@ -2124,7 +2184,7 @@
         <v>2021</v>
       </c>
       <c r="I14" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J14" s="11" t="s">
@@ -2144,11 +2204,11 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Comics_WarMachine</v>
       </c>
       <c r="B15" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>No</v>
       </c>
       <c r="C15" t="s">
@@ -2161,7 +2221,7 @@
         <v>2021</v>
       </c>
       <c r="I15" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J15" s="11" t="s">
@@ -2181,11 +2241,11 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_AbbysView</v>
       </c>
       <c r="B16" s="14" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>No</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -2201,7 +2261,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J16" s="11" t="s">
@@ -2224,11 +2284,11 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_Balance</v>
       </c>
       <c r="B17" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>No</v>
       </c>
       <c r="C17" t="s">
@@ -2239,7 +2299,7 @@
       </c>
       <c r="F17" s="10"/>
       <c r="I17" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J17" s="11" t="s">
@@ -2259,11 +2319,11 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_LaLunaDellamore</v>
       </c>
       <c r="B18" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>No</v>
       </c>
       <c r="C18" t="s">
@@ -2274,7 +2334,7 @@
       </c>
       <c r="F18" s="10"/>
       <c r="I18" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J18" s="11" t="s">
@@ -2294,11 +2354,11 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_LunarLove</v>
       </c>
       <c r="B19" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>No</v>
       </c>
       <c r="C19" t="s">
@@ -2309,7 +2369,7 @@
       </c>
       <c r="F19" s="10"/>
       <c r="I19" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J19" s="11" t="s">
@@ -2329,11 +2389,11 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Abstract_Fusion</v>
       </c>
       <c r="B20" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C20" t="s">
@@ -2352,7 +2412,7 @@
         <v>48</v>
       </c>
       <c r="I20" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x48</v>
       </c>
       <c r="J20" s="11" t="s">
@@ -2376,11 +2436,11 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Abstract_Gravity</v>
       </c>
       <c r="B21" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C21" t="s">
@@ -2399,7 +2459,7 @@
         <v>48</v>
       </c>
       <c r="I21" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x48</v>
       </c>
       <c r="J21" s="11" t="s">
@@ -2430,11 +2490,11 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Abstract_Power</v>
       </c>
       <c r="B22" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C22" t="s">
@@ -2453,7 +2513,7 @@
         <v>48</v>
       </c>
       <c r="I22" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x48</v>
       </c>
       <c r="J22" s="11" t="s">
@@ -2477,11 +2537,11 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Abstract_Samuri</v>
       </c>
       <c r="B23" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C23" t="s">
@@ -2500,7 +2560,7 @@
         <v>24</v>
       </c>
       <c r="I23" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J23" s="11" t="s">
@@ -2527,11 +2587,11 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Abstract_Suspension</v>
       </c>
       <c r="B24" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C24" t="s">
@@ -2550,7 +2610,7 @@
         <v>48</v>
       </c>
       <c r="I24" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x48</v>
       </c>
       <c r="J24" s="11" t="s">
@@ -2577,11 +2637,11 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_Ace</v>
       </c>
       <c r="B25" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C25" t="s">
@@ -2603,7 +2663,7 @@
         <v>36</v>
       </c>
       <c r="I25" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>30x36</v>
       </c>
       <c r="J25" s="11" t="s">
@@ -2634,11 +2694,11 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_ArabianPoetry</v>
       </c>
       <c r="B26" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C26" t="s">
@@ -2660,7 +2720,7 @@
         <v>48</v>
       </c>
       <c r="I26" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>36x48</v>
       </c>
       <c r="J26" s="11" t="s">
@@ -2689,11 +2749,11 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_Caution</v>
       </c>
       <c r="B27" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C27" t="s">
@@ -2715,7 +2775,7 @@
         <v>24</v>
       </c>
       <c r="I27" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J27" s="11" t="s">
@@ -2744,11 +2804,11 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_Chillin</v>
       </c>
       <c r="B28" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C28" t="s">
@@ -2761,7 +2821,7 @@
         <v>2020</v>
       </c>
       <c r="I28" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J28" s="11" t="s">
@@ -2781,11 +2841,11 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_Courage</v>
       </c>
       <c r="B29" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C29" t="s">
@@ -2807,7 +2867,7 @@
         <v>60</v>
       </c>
       <c r="I29" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x60</v>
       </c>
       <c r="J29" s="11" t="s">
@@ -2840,11 +2900,11 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_Curiosity</v>
       </c>
       <c r="B30" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C30" t="s">
@@ -2857,7 +2917,7 @@
         <v>2020</v>
       </c>
       <c r="I30" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J30" s="11" t="s">
@@ -2880,11 +2940,11 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_ErnieAndOakley</v>
       </c>
       <c r="B31" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C31" t="s">
@@ -2906,7 +2966,7 @@
         <v>30</v>
       </c>
       <c r="I31" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>30x30</v>
       </c>
       <c r="J31" s="11" t="s">
@@ -2939,11 +2999,11 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_Family</v>
       </c>
       <c r="B32" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C32" t="s">
@@ -2965,7 +3025,7 @@
         <v>40</v>
       </c>
       <c r="I32" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>30x40</v>
       </c>
       <c r="J32" s="11" t="s">
@@ -2994,11 +3054,11 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_FernandasPanther</v>
       </c>
       <c r="B33" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C33" t="s">
@@ -3020,7 +3080,7 @@
         <v>24</v>
       </c>
       <c r="I33" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x24</v>
       </c>
       <c r="J33" s="11" t="s">
@@ -3053,11 +3113,11 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_Focus</v>
       </c>
       <c r="B34" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C34" t="s">
@@ -3079,7 +3139,7 @@
         <v>24</v>
       </c>
       <c r="I34" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J34" s="11" t="s">
@@ -3108,11 +3168,11 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_Jewel</v>
       </c>
       <c r="B35" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C35" t="s">
@@ -3125,7 +3185,7 @@
         <v>2021</v>
       </c>
       <c r="I35" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J35" s="11" t="s">
@@ -3148,11 +3208,11 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_Jim</v>
       </c>
       <c r="B36" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C36" t="s">
@@ -3174,7 +3234,7 @@
         <v>36</v>
       </c>
       <c r="I36" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>30x36</v>
       </c>
       <c r="J36" s="11" t="s">
@@ -3207,11 +3267,11 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_LazyDay</v>
       </c>
       <c r="B37" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C37" t="s">
@@ -3233,7 +3293,7 @@
         <v>30</v>
       </c>
       <c r="I37" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x30</v>
       </c>
       <c r="J37" s="11" t="s">
@@ -3262,11 +3322,11 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_MyMilo</v>
       </c>
       <c r="B38" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C38" t="s">
@@ -3288,7 +3348,7 @@
         <v>30</v>
       </c>
       <c r="I38" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x30</v>
       </c>
       <c r="J38" s="11" t="s">
@@ -3317,11 +3377,11 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_MyPassion</v>
       </c>
       <c r="B39" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C39" t="s">
@@ -3343,7 +3403,7 @@
         <v>48</v>
       </c>
       <c r="I39" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>36x48</v>
       </c>
       <c r="J39" s="11" t="s">
@@ -3372,11 +3432,11 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_MyPippin</v>
       </c>
       <c r="B40" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C40" t="s">
@@ -3398,7 +3458,7 @@
         <v>24</v>
       </c>
       <c r="I40" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J40" s="11" t="s">
@@ -3429,11 +3489,11 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_Patience</v>
       </c>
       <c r="B41" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C41" t="s">
@@ -3455,7 +3515,7 @@
         <v>48</v>
       </c>
       <c r="I41" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>36x48</v>
       </c>
       <c r="J41" s="11" t="s">
@@ -3484,11 +3544,11 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_Shelter</v>
       </c>
       <c r="B42" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C42" t="s">
@@ -3501,7 +3561,7 @@
         <v>2021</v>
       </c>
       <c r="I42" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J42" s="11" t="s">
@@ -3526,11 +3586,11 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_TheSurvivor</v>
       </c>
       <c r="B43" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C43" t="s">
@@ -3552,7 +3612,7 @@
         <v>40</v>
       </c>
       <c r="I43" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>30x40</v>
       </c>
       <c r="J43" s="11" t="s">
@@ -3581,11 +3641,11 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Animals_Unleashed</v>
       </c>
       <c r="B44" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C44" t="s">
@@ -3607,7 +3667,7 @@
         <v>36</v>
       </c>
       <c r="I44" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>30x36</v>
       </c>
       <c r="J44" s="11" t="s">
@@ -3634,11 +3694,11 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Automotive_Ecto1</v>
       </c>
       <c r="B45" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C45" t="s">
@@ -3660,7 +3720,7 @@
         <v>36</v>
       </c>
       <c r="I45" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>30x36</v>
       </c>
       <c r="J45" s="11" t="s">
@@ -3687,11 +3747,11 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Automotive_IanLaw</v>
       </c>
       <c r="B46" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C46" t="s">
@@ -3713,7 +3773,7 @@
         <v>36</v>
       </c>
       <c r="I46" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>36x36</v>
       </c>
       <c r="J46" s="11" t="s">
@@ -3746,11 +3806,11 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Automotive_TimeMachine</v>
       </c>
       <c r="B47" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C47" t="s">
@@ -3772,7 +3832,7 @@
         <v>48</v>
       </c>
       <c r="I47" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>36x48</v>
       </c>
       <c r="J47" s="11" t="s">
@@ -3805,11 +3865,11 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Comics_Batman</v>
       </c>
       <c r="B48" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C48" t="s">
@@ -3831,7 +3891,7 @@
         <v>36</v>
       </c>
       <c r="I48" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x36</v>
       </c>
       <c r="J48" s="11" t="s">
@@ -3860,11 +3920,11 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Comics_EddieBrock</v>
       </c>
       <c r="B49" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C49" t="s">
@@ -3877,7 +3937,7 @@
         <v>2021</v>
       </c>
       <c r="I49" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J49" s="11" t="s">
@@ -3902,11 +3962,11 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Comics_Spiderman2000</v>
       </c>
       <c r="B50" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C50" t="s">
@@ -3928,7 +3988,7 @@
         <v>11</v>
       </c>
       <c r="I50" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>8x11</v>
       </c>
       <c r="J50" s="11" t="s">
@@ -3959,11 +4019,11 @@
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Comics_Spiderman2020</v>
       </c>
       <c r="B51" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C51" t="s">
@@ -3985,7 +4045,7 @@
         <v>48</v>
       </c>
       <c r="I51" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>36x48</v>
       </c>
       <c r="J51" s="11" t="s">
@@ -4014,11 +4074,11 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Comics_SpidermanMilesMorales</v>
       </c>
       <c r="B52" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C52" t="s">
@@ -4037,7 +4097,7 @@
         <v>36</v>
       </c>
       <c r="I52" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x36</v>
       </c>
       <c r="J52" s="11" t="s">
@@ -4070,11 +4130,11 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Comics_TheHulk</v>
       </c>
       <c r="B53" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C53" t="s">
@@ -4096,7 +4156,7 @@
         <v>36</v>
       </c>
       <c r="I53" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>30x36</v>
       </c>
       <c r="J53" s="11" t="s">
@@ -4127,11 +4187,11 @@
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Comics_Venom</v>
       </c>
       <c r="B54" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C54" t="s">
@@ -4150,7 +4210,7 @@
         <v>20</v>
       </c>
       <c r="I54" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>16x20</v>
       </c>
       <c r="J54" s="11" t="s">
@@ -4183,11 +4243,11 @@
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Comics_Waiting</v>
       </c>
       <c r="B55" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C55" t="s">
@@ -4209,7 +4269,7 @@
         <v>30</v>
       </c>
       <c r="I55" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>30x30</v>
       </c>
       <c r="J55" s="11" t="s">
@@ -4236,11 +4296,11 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_Afternoon</v>
       </c>
       <c r="B56" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C56" t="s">
@@ -4259,7 +4319,7 @@
         <v>16</v>
       </c>
       <c r="I56" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>14x16</v>
       </c>
       <c r="J56" s="11" t="s">
@@ -4286,11 +4346,11 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_AlgonquinTree</v>
       </c>
       <c r="B57" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C57" t="s">
@@ -4309,7 +4369,7 @@
         <v>24</v>
       </c>
       <c r="I57" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>18x24</v>
       </c>
       <c r="J57" s="11" t="s">
@@ -4338,11 +4398,11 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_ArizonaSunset</v>
       </c>
       <c r="B58" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C58" t="s">
@@ -4361,7 +4421,7 @@
         <v>20</v>
       </c>
       <c r="I58" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>16x20</v>
       </c>
       <c r="J58" s="11" t="s">
@@ -4390,11 +4450,11 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_AuroraBorealis</v>
       </c>
       <c r="B59" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C59" t="s">
@@ -4413,7 +4473,7 @@
         <v>30</v>
       </c>
       <c r="I59" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x30</v>
       </c>
       <c r="J59" s="11" t="s">
@@ -4442,11 +4502,11 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_AzielBackyard</v>
       </c>
       <c r="B60" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C60" t="s">
@@ -4468,7 +4528,7 @@
         <v>22</v>
       </c>
       <c r="I60" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>16x22</v>
       </c>
       <c r="J60" s="11" t="s">
@@ -4497,11 +4557,11 @@
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_Cabin</v>
       </c>
       <c r="B61" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C61" t="s">
@@ -4520,7 +4580,7 @@
         <v>16</v>
       </c>
       <c r="I61" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>14x16</v>
       </c>
       <c r="J61" s="11" t="s">
@@ -4547,11 +4607,11 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_CottageSunset</v>
       </c>
       <c r="B62" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C62" t="s">
@@ -4573,7 +4633,7 @@
         <v>24</v>
       </c>
       <c r="I62" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x24</v>
       </c>
       <c r="J62" s="11" t="s">
@@ -4600,11 +4660,11 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_CottageSunsetII</v>
       </c>
       <c r="B63" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C63" t="s">
@@ -4626,7 +4686,7 @@
         <v>24</v>
       </c>
       <c r="I63" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x24</v>
       </c>
       <c r="J63" s="11" t="s">
@@ -4659,11 +4719,11 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_CottageSunsetIII</v>
       </c>
       <c r="B64" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C64" t="s">
@@ -4685,7 +4745,7 @@
         <v>24</v>
       </c>
       <c r="I64" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x24</v>
       </c>
       <c r="J64" s="11" t="s">
@@ -4718,11 +4778,11 @@
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_DarkCastle</v>
       </c>
       <c r="B65" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C65" t="s">
@@ -4741,7 +4801,7 @@
         <v>16</v>
       </c>
       <c r="I65" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>14x16</v>
       </c>
       <c r="J65" s="11" t="s">
@@ -4768,11 +4828,11 @@
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_FallsInTheWoods</v>
       </c>
       <c r="B66" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C66" t="s">
@@ -4791,7 +4851,7 @@
         <v>24</v>
       </c>
       <c r="I66" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J66" s="11" t="s">
@@ -4820,11 +4880,11 @@
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_Floating</v>
       </c>
       <c r="B67" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C67" t="s">
@@ -4843,7 +4903,7 @@
         <v>48</v>
       </c>
       <c r="I67" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x48</v>
       </c>
       <c r="J67" s="11" t="s">
@@ -4872,11 +4932,11 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_Footbridge</v>
       </c>
       <c r="B68" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C68" t="s">
@@ -4895,7 +4955,7 @@
         <v>16</v>
       </c>
       <c r="I68" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>14x16</v>
       </c>
       <c r="J68" s="11" t="s">
@@ -4922,11 +4982,11 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_LighthouseCliffs</v>
       </c>
       <c r="B69" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C69" t="s">
@@ -4945,7 +5005,7 @@
         <v>24</v>
       </c>
       <c r="I69" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x24</v>
       </c>
       <c r="J69" s="11" t="s">
@@ -4972,11 +5032,11 @@
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_MainStreetMountAlbert</v>
       </c>
       <c r="B70" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C70" t="s">
@@ -4998,7 +5058,7 @@
         <v>24</v>
       </c>
       <c r="I70" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>18x24</v>
       </c>
       <c r="J70" s="11" t="s">
@@ -5025,11 +5085,11 @@
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_Meadow</v>
       </c>
       <c r="B71" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C71" t="s">
@@ -5048,7 +5108,7 @@
         <v>24</v>
       </c>
       <c r="I71" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>18x24</v>
       </c>
       <c r="J71" s="11" t="s">
@@ -5081,11 +5141,11 @@
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_Mountains</v>
       </c>
       <c r="B72" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C72" t="s">
@@ -5104,7 +5164,7 @@
         <v>24</v>
       </c>
       <c r="I72" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>18x24</v>
       </c>
       <c r="J72" s="11" t="s">
@@ -5131,11 +5191,11 @@
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_NiagaraFalls</v>
       </c>
       <c r="B73" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C73" t="s">
@@ -5154,7 +5214,7 @@
         <v>36</v>
       </c>
       <c r="I73" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>36x36</v>
       </c>
       <c r="J73" s="11" t="s">
@@ -5183,11 +5243,11 @@
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_OnTheRoadAgain</v>
       </c>
       <c r="B74" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C74" t="s">
@@ -5206,7 +5266,7 @@
         <v>18</v>
       </c>
       <c r="I74" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>14x18</v>
       </c>
       <c r="J74" s="11" t="s">
@@ -5233,11 +5293,11 @@
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_Paradise</v>
       </c>
       <c r="B75" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C75" t="s">
@@ -5256,7 +5316,7 @@
         <v>42</v>
       </c>
       <c r="I75" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>26x42</v>
       </c>
       <c r="J75" s="11" t="s">
@@ -5285,11 +5345,11 @@
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_PathInTheWoods</v>
       </c>
       <c r="B76" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C76" t="s">
@@ -5308,7 +5368,7 @@
         <v>24</v>
       </c>
       <c r="I76" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>18x24</v>
       </c>
       <c r="J76" s="11" t="s">
@@ -5335,11 +5395,11 @@
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_PathThroughTheWoods</v>
       </c>
       <c r="B77" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C77" t="s">
@@ -5358,7 +5418,7 @@
         <v>48</v>
       </c>
       <c r="I77" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>36x48</v>
       </c>
       <c r="J77" s="11" t="s">
@@ -5385,11 +5445,11 @@
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_PortlandLighthouse</v>
       </c>
       <c r="B78" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C78" t="s">
@@ -5408,7 +5468,7 @@
         <v>24</v>
       </c>
       <c r="I78" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J78" s="11" t="s">
@@ -5441,11 +5501,11 @@
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_Reflections</v>
       </c>
       <c r="B79" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C79" t="s">
@@ -5464,7 +5524,7 @@
         <v>30</v>
       </c>
       <c r="I79" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x30</v>
       </c>
       <c r="J79" s="11" t="s">
@@ -5493,11 +5553,11 @@
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_SailorsDelight</v>
       </c>
       <c r="B80" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C80" t="s">
@@ -5516,7 +5576,7 @@
         <v>30</v>
       </c>
       <c r="I80" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>30x30</v>
       </c>
       <c r="J80" s="11" t="s">
@@ -5545,11 +5605,11 @@
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_SummerOnACountryRoad</v>
       </c>
       <c r="B81" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C81" t="s">
@@ -5568,7 +5628,7 @@
         <v>24</v>
       </c>
       <c r="I81" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>18x24</v>
       </c>
       <c r="J81" s="11" t="s">
@@ -5601,11 +5661,11 @@
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_Sunlight</v>
       </c>
       <c r="B82" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C82" t="s">
@@ -5624,7 +5684,7 @@
         <v>48</v>
       </c>
       <c r="I82" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>36x48</v>
       </c>
       <c r="J82" s="11" t="s">
@@ -5653,11 +5713,11 @@
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_SunsetOnMajikFarm</v>
       </c>
       <c r="B83" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C83" t="s">
@@ -5679,7 +5739,7 @@
         <v>24</v>
       </c>
       <c r="I83" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>18x24</v>
       </c>
       <c r="J83" s="11" t="s">
@@ -5708,11 +5768,11 @@
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_SunsetThroughTheGlades</v>
       </c>
       <c r="B84" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C84" t="s">
@@ -5731,7 +5791,7 @@
         <v>30</v>
       </c>
       <c r="I84" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>30x30</v>
       </c>
       <c r="J84" s="11" t="s">
@@ -5758,11 +5818,11 @@
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_TheGarden</v>
       </c>
       <c r="B85" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C85" t="s">
@@ -5781,7 +5841,7 @@
         <v>33</v>
       </c>
       <c r="I85" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>27x33</v>
       </c>
       <c r="J85" s="11" t="s">
@@ -5810,11 +5870,11 @@
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_TheOldMill</v>
       </c>
       <c r="B86" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C86" t="s">
@@ -5836,7 +5896,7 @@
         <v>30</v>
       </c>
       <c r="I86" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x30</v>
       </c>
       <c r="J86" s="11" t="s">
@@ -5865,11 +5925,11 @@
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_TrainBridge</v>
       </c>
       <c r="B87" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C87" t="s">
@@ -5888,7 +5948,7 @@
         <v>16</v>
       </c>
       <c r="I87" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>14x16</v>
       </c>
       <c r="J87" s="11" t="s">
@@ -5915,11 +5975,11 @@
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_TrainBridgeII</v>
       </c>
       <c r="B88" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C88" t="s">
@@ -5938,7 +5998,7 @@
         <v>24</v>
       </c>
       <c r="I88" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x24</v>
       </c>
       <c r="J88" s="11" t="s">
@@ -5965,11 +6025,11 @@
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Landscape_WardenAndMountAlbert</v>
       </c>
       <c r="B89" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C89" t="s">
@@ -5991,7 +6051,7 @@
         <v>30</v>
       </c>
       <c r="I89" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x30</v>
       </c>
       <c r="J89" s="11" t="s">
@@ -6020,11 +6080,11 @@
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_Alexandra</v>
       </c>
       <c r="B90" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C90" t="s">
@@ -6046,7 +6106,7 @@
         <v>24</v>
       </c>
       <c r="I90" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x24</v>
       </c>
       <c r="J90" s="11" t="s">
@@ -6079,11 +6139,11 @@
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_Angel1</v>
       </c>
       <c r="B91" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C91" t="s">
@@ -6105,7 +6165,7 @@
         <v>24</v>
       </c>
       <c r="I91" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J91" s="11" t="s">
@@ -6136,11 +6196,11 @@
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_Angel2</v>
       </c>
       <c r="B92" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C92" t="s">
@@ -6162,7 +6222,7 @@
         <v>24</v>
       </c>
       <c r="I92" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J92" s="11" t="s">
@@ -6193,11 +6253,11 @@
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_Angel3</v>
       </c>
       <c r="B93" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C93" t="s">
@@ -6219,7 +6279,7 @@
         <v>24</v>
       </c>
       <c r="I93" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J93" s="11" t="s">
@@ -6250,11 +6310,11 @@
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A94" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_ChanelWestCoast</v>
       </c>
       <c r="B94" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C94" t="s">
@@ -6276,7 +6336,7 @@
         <v>24</v>
       </c>
       <c r="I94" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J94" s="11" t="s">
@@ -6305,11 +6365,11 @@
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A95" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_Edward</v>
       </c>
       <c r="B95" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C95" t="s">
@@ -6331,7 +6391,7 @@
         <v>24</v>
       </c>
       <c r="I95" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J95" s="11" t="s">
@@ -6364,11 +6424,11 @@
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A96" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_HenrysMirror</v>
       </c>
       <c r="B96" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C96" t="s">
@@ -6381,7 +6441,7 @@
         <v>2021</v>
       </c>
       <c r="I96" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>x</v>
       </c>
       <c r="J96" s="11" t="s">
@@ -6412,11 +6472,11 @@
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_LadyInRed</v>
       </c>
       <c r="B97" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C97" t="s">
@@ -6438,7 +6498,7 @@
         <v>24</v>
       </c>
       <c r="I97" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x24</v>
       </c>
       <c r="J97" s="11" t="s">
@@ -6467,11 +6527,11 @@
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_LoveAtFirstSight</v>
       </c>
       <c r="B98" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C98" t="s">
@@ -6493,7 +6553,7 @@
         <v>30</v>
       </c>
       <c r="I98" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x30</v>
       </c>
       <c r="J98" s="11" t="s">
@@ -6522,11 +6582,11 @@
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A99" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_MattDematteo</v>
       </c>
       <c r="B99" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C99" t="s">
@@ -6548,7 +6608,7 @@
         <v>24</v>
       </c>
       <c r="I99" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J99" s="11" t="s">
@@ -6581,11 +6641,11 @@
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A100" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_MyDustin</v>
       </c>
       <c r="B100" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C100" t="s">
@@ -6607,7 +6667,7 @@
         <v>24</v>
       </c>
       <c r="I100" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J100" s="11" t="s">
@@ -6633,11 +6693,11 @@
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A101" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_MyDustinII</v>
       </c>
       <c r="B101" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C101" t="s">
@@ -6659,7 +6719,7 @@
         <v>24</v>
       </c>
       <c r="I101" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J101" s="11" t="s">
@@ -6685,11 +6745,11 @@
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_MyMonika</v>
       </c>
       <c r="B102" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C102" t="s">
@@ -6711,7 +6771,7 @@
         <v>24</v>
       </c>
       <c r="I102" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J102" s="11" t="s">
@@ -6740,11 +6800,11 @@
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A103" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_MyPrincess</v>
       </c>
       <c r="B103" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C103" t="s">
@@ -6766,7 +6826,7 @@
         <v>24</v>
       </c>
       <c r="I103" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J103" s="11" t="s">
@@ -6797,11 +6857,11 @@
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_MyRussell</v>
       </c>
       <c r="B104" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C104" t="s">
@@ -6823,7 +6883,7 @@
         <v>24</v>
       </c>
       <c r="I104" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x24</v>
       </c>
       <c r="J104" s="11" t="s">
@@ -6852,11 +6912,11 @@
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A105" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_Myself</v>
       </c>
       <c r="B105" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C105" t="s">
@@ -6878,7 +6938,7 @@
         <v>24</v>
       </c>
       <c r="I105" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J105" s="11" t="s">
@@ -6907,11 +6967,11 @@
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_MyTyler</v>
       </c>
       <c r="B106" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C106" t="s">
@@ -6933,7 +6993,7 @@
         <v>20</v>
       </c>
       <c r="I106" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>16x20</v>
       </c>
       <c r="J106" s="11" t="s">
@@ -6962,11 +7022,11 @@
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_MyTylerII</v>
       </c>
       <c r="B107" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C107" t="s">
@@ -6988,7 +7048,7 @@
         <v>24</v>
       </c>
       <c r="I107" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J107" s="11" t="s">
@@ -7017,11 +7077,11 @@
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_MyZachary</v>
       </c>
       <c r="B108" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C108" t="s">
@@ -7043,7 +7103,7 @@
         <v>24</v>
       </c>
       <c r="I108" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J108" s="11" t="s">
@@ -7072,11 +7132,11 @@
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A109" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_MyZacharyII</v>
       </c>
       <c r="B109" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C109" t="s">
@@ -7098,7 +7158,7 @@
         <v>24</v>
       </c>
       <c r="I109" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J109" s="11" t="s">
@@ -7127,11 +7187,11 @@
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_Sammy</v>
       </c>
       <c r="B110" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C110" t="s">
@@ -7153,7 +7213,7 @@
         <v>36</v>
       </c>
       <c r="I110" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>30x36</v>
       </c>
       <c r="J110" s="11" t="s">
@@ -7180,11 +7240,11 @@
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A111" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_Terra</v>
       </c>
       <c r="B111" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C111" t="s">
@@ -7206,7 +7266,7 @@
         <v>24</v>
       </c>
       <c r="I111" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J111" s="11" t="s">
@@ -7239,11 +7299,11 @@
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Portrait_TheWiseWoman</v>
       </c>
       <c r="B112" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C112" t="s">
@@ -7265,7 +7325,7 @@
         <v>24</v>
       </c>
       <c r="I112" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>20x24</v>
       </c>
       <c r="J112" s="11" t="s">
@@ -7294,11 +7354,11 @@
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A113" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Sports_Dustin</v>
       </c>
       <c r="B113" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C113" t="s">
@@ -7320,7 +7380,7 @@
         <v>20</v>
       </c>
       <c r="I113" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>14x20</v>
       </c>
       <c r="J113" s="11" t="s">
@@ -7351,11 +7411,11 @@
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Sports_Jockeys</v>
       </c>
       <c r="B114" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C114" t="s">
@@ -7377,7 +7437,7 @@
         <v>36</v>
       </c>
       <c r="I114" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>36x36</v>
       </c>
       <c r="J114" s="11" t="s">
@@ -7406,11 +7466,11 @@
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Sports_LesleyWithTimberSpirit</v>
       </c>
       <c r="B115" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C115" t="s">
@@ -7432,7 +7492,7 @@
         <v>20</v>
       </c>
       <c r="I115" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>14x20</v>
       </c>
       <c r="J115" s="11" t="s">
@@ -7461,11 +7521,11 @@
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Sports_PaulCoffey</v>
       </c>
       <c r="B116" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C116" t="s">
@@ -7487,7 +7547,7 @@
         <v>20</v>
       </c>
       <c r="I116" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>16x20</v>
       </c>
       <c r="J116" s="11" t="s">
@@ -7516,11 +7576,11 @@
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Sports_TheGreatOne</v>
       </c>
       <c r="B117" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C117" t="s">
@@ -7542,7 +7602,7 @@
         <v>20</v>
       </c>
       <c r="I117" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>16x20</v>
       </c>
       <c r="J117" s="11" t="s">
@@ -7571,11 +7631,11 @@
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Sports_Tyler</v>
       </c>
       <c r="B118" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C118" t="s">
@@ -7597,7 +7657,7 @@
         <v>20</v>
       </c>
       <c r="I118" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>14x20</v>
       </c>
       <c r="J118" s="11" t="s">
@@ -7628,11 +7688,11 @@
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A119" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Sports_Zack</v>
       </c>
       <c r="B119" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C119" t="s">
@@ -7654,7 +7714,7 @@
         <v>20</v>
       </c>
       <c r="I119" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>14x20</v>
       </c>
       <c r="J119" s="11" t="s">
@@ -7685,11 +7745,11 @@
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A120" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Stills_Hydrangeas</v>
       </c>
       <c r="B120" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C120" t="s">
@@ -7711,7 +7771,7 @@
         <v>24</v>
       </c>
       <c r="I120" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>24x24</v>
       </c>
       <c r="J120" s="11" t="s">
@@ -7740,11 +7800,11 @@
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A121" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Stills_IvyGeraniums</v>
       </c>
       <c r="B121" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C121" t="s">
@@ -7766,7 +7826,7 @@
         <v>16</v>
       </c>
       <c r="I121" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>16x16</v>
       </c>
       <c r="J121" s="11" t="s">
@@ -7795,11 +7855,11 @@
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A122" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Stills_Mistletoe</v>
       </c>
       <c r="B122" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C122" t="s">
@@ -7821,7 +7881,7 @@
         <v>16</v>
       </c>
       <c r="I122" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>14x16</v>
       </c>
       <c r="J122" s="11" t="s">
@@ -7848,11 +7908,11 @@
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A123" s="9" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Stills_Roses</v>
       </c>
       <c r="B123" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C123" t="s">
@@ -7874,7 +7934,7 @@
         <v>16</v>
       </c>
       <c r="I123" s="8" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>14x16</v>
       </c>
       <c r="J123" s="11" t="s">
@@ -7907,11 +7967,11 @@
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A124" s="4" t="str">
-        <f>SUBSTITUTE((_xlfn.CONCAT(Paintings.Table[[#This Row],[Category]],"_",Paintings.Table[[#This Row],[Title]]))," ","")</f>
+        <f>SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ","")</f>
         <v>Stills_WallOfRoses</v>
       </c>
       <c r="B124" s="12" t="str">
-        <f>IF(Paintings.Table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
+        <f>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C124" t="s">
@@ -7933,7 +7993,7 @@
         <v>28</v>
       </c>
       <c r="I124" s="5" t="str">
-        <f>_xlfn.CONCAT(Paintings.Table[[#This Row],[Width]],"x",Paintings.Table[[#This Row],[Length]])</f>
+        <f>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</f>
         <v>22x28</v>
       </c>
       <c r="J124" s="11" t="s">
@@ -7962,11 +8022,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="expression" dxfId="18" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$P1="Edit Post"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$Q1="Absent"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:R124">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>$O2="SOLD"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">

</xml_diff>

<commit_message>
updated photos for portfolio
</commit_message>
<xml_diff>
--- a/docs/portfolio.xlsx
+++ b/docs/portfolio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ecc85ccb002dd88c/Projects/mooremanordesigns.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="736" documentId="13_ncr:1_{F5B818F5-FA86-4F87-A408-A48E3EF64669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3413ED90-1C71-481B-8624-01183B5E0317}"/>
+  <xr:revisionPtr revIDLastSave="737" documentId="13_ncr:1_{F5B818F5-FA86-4F87-A408-A48E3EF64669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2D3FA20-04C1-4998-A59A-A0C8594121A7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{436361DF-52DD-460D-9FB3-3363FA009BCD}"/>
   </bookViews>
@@ -1288,44 +1288,15 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="28">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
@@ -1355,16 +1326,6 @@
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1376,9 +1337,9 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="solid">
+        <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1393,11 +1354,14 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1419,8 +1383,10 @@
     </dxf>
     <dxf>
       <font>
-        <i/>
+        <b val="0"/>
+        <i val="0"/>
       </font>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1441,13 +1407,9 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
+      <font>
+        <i/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -1458,19 +1420,7 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1503,16 +1453,53 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1527,10 +1514,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/namedSheetViews/namedSheetView1.xml><?xml version="1.0" encoding="utf-8"?>
-<namedSheetViews xmlns="http://schemas.microsoft.com/office/spreadsheetml/2019/namedsheetviews" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Zachary Moore" id="{1ADAE229-958C-465B-924E-E3BF28E593DD}" userId="Zachary Moore" providerId="None"/>
@@ -1538,35 +1521,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BEC4E9FD-2B38-4FC7-8049-9023C5F715E4}" name="portfolio.table" displayName="portfolio.table" ref="A1:R139" headerRowDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BEC4E9FD-2B38-4FC7-8049-9023C5F715E4}" name="portfolio.table" displayName="portfolio.table" ref="A1:R139" headerRowDxfId="24">
   <autoFilter ref="A1:R139" xr:uid="{23143FBE-2AF4-46A6-9F78-52A9759D713F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R139">
     <sortCondition ref="A1:A139"/>
   </sortState>
   <tableColumns count="18">
-    <tableColumn id="9" xr3:uid="{5B7A858D-E5C0-47C8-95F1-29BE364D59D1}" name="Filename" totalsRowLabel="Total" dataDxfId="23" totalsRowDxfId="24">
+    <tableColumn id="9" xr3:uid="{5B7A858D-E5C0-47C8-95F1-29BE364D59D1}" name="Filename" totalsRowLabel="Total" dataDxfId="23" totalsRowDxfId="22">
       <calculatedColumnFormula>HYPERLINK(_xlfn.CONCAT("C:/Users/zack_/OneDrive/Projects/mooremanordesigns.github.io/portfolio_org/",SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ",""),".jpg"),SUBSTITUTE((_xlfn.CONCAT(portfolio.table[[#This Row],[Category]],"_",portfolio.table[[#This Row],[Title]]))," ",""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{1C22BD59-9C25-4F2C-8884-72C883A837B1}" name="Include" dataDxfId="21" totalsRowDxfId="22">
+    <tableColumn id="14" xr3:uid="{1C22BD59-9C25-4F2C-8884-72C883A837B1}" name="Include" dataDxfId="21" totalsRowDxfId="20">
       <calculatedColumnFormula>IF(portfolio.table[[#This Row],[Status.Photo]]="Absent","No","Yes")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="1" xr3:uid="{7DF0D842-9A07-4F32-9A22-C88E5853ED33}" name="Category"/>
     <tableColumn id="2" xr3:uid="{BC061CA4-BDC5-44BA-B403-ACD105A38E6A}" name="Series"/>
-    <tableColumn id="3" xr3:uid="{B7D64594-94CF-4D23-B1E1-CF59D686B1F3}" name="Title" dataDxfId="19" totalsRowDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{4D7F8670-91BB-40FA-B49C-62566B0B2CAB}" name="Year" dataDxfId="17" totalsRowDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{B7D64594-94CF-4D23-B1E1-CF59D686B1F3}" name="Title" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{4D7F8670-91BB-40FA-B49C-62566B0B2CAB}" name="Year" dataDxfId="17" totalsRowDxfId="16"/>
     <tableColumn id="4" xr3:uid="{3F8A6B28-1093-4693-9FF7-6105AED8534B}" name="Width"/>
     <tableColumn id="5" xr3:uid="{72C2B875-E7D6-4BB5-9FE4-1B38EF88FD7B}" name="Length"/>
-    <tableColumn id="6" xr3:uid="{86825EB6-C340-453B-A16A-48B0274F4965}" name="Dimensions" dataDxfId="15" totalsRowDxfId="16">
+    <tableColumn id="6" xr3:uid="{86825EB6-C340-453B-A16A-48B0274F4965}" name="Dimensions" dataDxfId="15" totalsRowDxfId="14">
       <calculatedColumnFormula>_xlfn.CONCAT(portfolio.table[[#This Row],[Width]],"x",portfolio.table[[#This Row],[Length]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{D204B81F-B1E3-4F84-9E11-6A7F96BA5521}" name="Framed" dataDxfId="13" totalsRowDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{CF043A25-5602-4987-9A50-FBE0E6A6FF6D}" name="Price.Ask" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="12"/>
-    <tableColumn id="12" xr3:uid="{649C86E1-9495-4246-BAC2-CED30A646F0F}" name="Price.Sale" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="10"/>
-    <tableColumn id="15" xr3:uid="{F2298965-3AF1-4CB7-A947-2BC83C4B3530}" name="Status.Notes" dataDxfId="8"/>
-    <tableColumn id="20" xr3:uid="{63861CEA-B9F4-4389-804D-5B6F1F0BFE89}" name="Sale.Date" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{836D4801-5D71-4595-97A7-D202ACE67724}" name="Status.Sale" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{0715EB14-7918-456A-8D07-251FC53FEF2B}" name="Status.Info" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{C475F84E-A8C2-4675-96A9-370E4BE697BD}" name="Status.Photo" dataDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{D204B81F-B1E3-4F84-9E11-6A7F96BA5521}" name="Framed" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{CF043A25-5602-4987-9A50-FBE0E6A6FF6D}" name="Price.Ask" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{649C86E1-9495-4246-BAC2-CED30A646F0F}" name="Price.Sale" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{F2298965-3AF1-4CB7-A947-2BC83C4B3530}" name="Status.Notes" dataDxfId="7"/>
+    <tableColumn id="20" xr3:uid="{63861CEA-B9F4-4389-804D-5B6F1F0BFE89}" name="Sale.Date" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{836D4801-5D71-4595-97A7-D202ACE67724}" name="Status.Sale" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{0715EB14-7918-456A-8D07-251FC53FEF2B}" name="Status.Info" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{C475F84E-A8C2-4675-96A9-370E4BE697BD}" name="Status.Photo" dataDxfId="3"/>
     <tableColumn id="10" xr3:uid="{5326519F-F06A-4075-A35A-AA69D194CDB1}" name="Description" totalsRowFunction="count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1574,7 +1557,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5DDE0F4D-CD7D-42F0-AAD4-99E4FD427C88}" name="Category.Table" displayName="Category.Table" ref="A2:A10" totalsRowShown="0" headerRowDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5DDE0F4D-CD7D-42F0-AAD4-99E4FD427C88}" name="Category.Table" displayName="Category.Table" ref="A2:A10" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A2:A10" xr:uid="{535629D5-D5B3-4151-81E7-AC9A74A5ED01}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A8">
     <sortCondition ref="A2:A8"/>
@@ -1587,7 +1570,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7802B257-70CD-41BB-AFBF-5480702F402C}" name="Subcategory.Table" displayName="Subcategory.Table" ref="C2:I8" totalsRowShown="0" headerRowDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7802B257-70CD-41BB-AFBF-5480702F402C}" name="Subcategory.Table" displayName="Subcategory.Table" ref="C2:I8" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="C2:I8" xr:uid="{08463D02-E487-4EEB-A80C-CA4F702068E6}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{A1231EA8-3C3E-4975-B930-61C0B93A50E2}" name="Portait"/>
@@ -1603,7 +1586,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BBDF68BD-D421-487E-94D4-D0F9FDD9892F}" name="Status.Table" displayName="Status.Table" ref="K2:M9" totalsRowShown="0" headerRowDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BBDF68BD-D421-487E-94D4-D0F9FDD9892F}" name="Status.Table" displayName="Status.Table" ref="K2:M9" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="K2:M9" xr:uid="{7597EB04-335A-4658-9C5E-54700C2640F3}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E3C3437E-D4C6-46B5-A846-07B0F64A27ED}" name="Status.Sale"/>
@@ -1923,13 +1906,13 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E8" sqref="E8"/>
+      <selection pane="topRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.6640625" customWidth="1"/>
-    <col min="2" max="2" width="8.21875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="8.21875" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="14.5546875" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
@@ -1944,8 +1927,7 @@
     <col min="16" max="16" width="7" customWidth="1"/>
     <col min="17" max="17" width="7.44140625" customWidth="1"/>
     <col min="18" max="18" width="51.33203125" customWidth="1"/>
-    <col min="19" max="19" width="41" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="41" hidden="1"/>
+    <col min="19" max="20" width="41" hidden="1" customWidth="1"/>
     <col min="21" max="16384" width="27.5546875" hidden="1"/>
   </cols>
   <sheetData>
@@ -9393,15 +9375,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="27" priority="1">
       <formula>$Q1="Absent"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="26" priority="2">
       <formula>$P1="Edit"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:R139">
-    <cfRule type="expression" dxfId="0" priority="4">
+    <cfRule type="expression" dxfId="25" priority="4">
       <formula>OR($O2="COMMISSIONED",$O2="SOLD",$O2="GIFTED",$O2="OTHER")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>